<commit_message>
Updated the reference number for the UART Mux for the correct footprint
</commit_message>
<xml_diff>
--- a/IRIS2/01-Design/IRIS2_PCB_CPU/Project Outputs for IRIS2_PCB_CPU/20210415_IRIS2_PCB_CPU_BOM.xlsx
+++ b/IRIS2/01-Design/IRIS2_PCB_CPU/Project Outputs for IRIS2_PCB_CPU/20210415_IRIS2_PCB_CPU_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bultz\workspace_daedalus\IRIS2\IRIS2\01-Design\IRIS2_PCB_CPU\Project Outputs for IRIS2_PCB_CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4E1242-7C82-4DAE-8F11-F6FEBF6857A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AFEBFC-5429-4076-8D01-19C4A7C9E76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="2610" windowWidth="21600" windowHeight="12735" xr2:uid="{97345CF3-A20C-4F64-8EBE-6094E00D78B9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{97345CF3-A20C-4F64-8EBE-6094E00D78B9}"/>
   </bookViews>
   <sheets>
     <sheet name="20210415_IRIS2_PCB_CPU_BOM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="126">
   <si>
     <t>Designator</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>INA226AQDGSRQ1</t>
+  </si>
+  <si>
+    <t>PI3USB221AZUAEX</t>
   </si>
 </sst>
 </file>
@@ -800,8 +803,8 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,7 +1476,7 @@
         <v>118</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>119</v>

</xml_diff>